<commit_message>
Update and improve cModelTable
- Updates cModelTable with improved validation, adds detailed field and sample checks.
- Enhances cParseStream with duplicate and invalid key/name detection.
- Updates cType with DataType struct.
- Removes old datamodel_config.json files and updates JSON schema definitions and example files for consistency with new validation logic.
</commit_message>
<xml_diff>
--- a/Examples/cgam/prueba.xlsx
+++ b/Examples/cgam/prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\cgam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E64D21-3F9D-4796-BFBA-1BDCA90CEED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7757219A-49F2-47AF-B4CE-1A07CF30C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28410" yWindow="-885" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="780" windowWidth="25740" windowHeight="14700" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Exergy" sheetId="3" r:id="rId5"/>
     <sheet name="Format" sheetId="6" r:id="rId6"/>
     <sheet name="WasteDefinition" sheetId="8" r:id="rId7"/>
-    <sheet name="WasteAllocationx" sheetId="10" r:id="rId8"/>
+    <sheet name="WasteAllocation" sheetId="10" r:id="rId8"/>
     <sheet name="ResourcesCost" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
@@ -100,8 +100,30 @@
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
   <si>
     <t>key</t>
   </si>
@@ -402,9 +424,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -414,6 +435,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,16 +840,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -890,121 +917,124 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1025,7 +1055,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,19 +1070,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1159,6 +1189,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1180,7 +1211,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,59 +1220,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="str">
+      <c r="A1" s="2" t="str">
         <f>Flows!A1</f>
         <v>key</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
+      <c r="A2" s="2" t="str">
         <f>Flows!A2</f>
         <v>NG</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>72.465000000000003</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>73.326999999999998</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>73.599999999999994</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>73.296999999999997</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>72.283000000000001</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>72.465000000000003</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>72.465000000000003</v>
       </c>
       <c r="I2">
@@ -1249,29 +1280,29 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="str">
+      <c r="A3" s="2" t="str">
         <f>Flows!A3</f>
         <v>B1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="I3">
@@ -1279,29 +1310,29 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="str">
+      <c r="A4" s="2" t="str">
         <f>Flows!A4</f>
         <v>B2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>28.651</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>29.507000000000001</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>29.337</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>29.196000000000002</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>27.863</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>28.651</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>28.651</v>
       </c>
       <c r="I4">
@@ -1309,29 +1340,29 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="2" t="str">
         <f>Flows!A5</f>
         <v>B3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>50.338999999999999</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>50.896000000000001</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>51.926000000000002</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>51.018000000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>51.048000000000002</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>50.338999999999999</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>50.338999999999999</v>
       </c>
       <c r="I5">
@@ -1339,29 +1370,29 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="2" t="str">
         <f>Flows!A6</f>
         <v>B4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>102.53</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>103.462</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>104.971</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>103.813</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>103.163</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>102.53</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>102.53</v>
       </c>
       <c r="I6">
@@ -1369,29 +1400,29 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="2" t="str">
         <f>Flows!A7</f>
         <v>B5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>38.81</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>38.734999999999999</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>40.229999999999997</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>39.295000000000002</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>40.323999999999998</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>38.81</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>38.81</v>
       </c>
       <c r="I7">
@@ -1399,29 +1430,29 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="str">
+      <c r="A8" s="2" t="str">
         <f>Flows!A8</f>
         <v>B6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>14.784000000000001</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>15.021000000000001</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>15.212999999999999</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>15.137</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>14.597</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>14.784000000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>14.784000000000001</v>
       </c>
       <c r="I8">
@@ -1429,29 +1460,29 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="2" t="str">
         <f>Flows!A9</f>
         <v>B7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>2.1219999999999999</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>2.23</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>2.1560000000000001</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>2.1120000000000001</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>2.2280000000000002</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>2.3530000000000002</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>14.784000000000001</v>
       </c>
       <c r="I9">
@@ -1459,29 +1490,29 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="str">
+      <c r="A10" s="2" t="str">
         <f>Flows!A10</f>
         <v>WC</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>31.105</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>32.033000000000001</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>31.849</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>31.869</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>30.295000000000002</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>31.105</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>31.105</v>
       </c>
       <c r="I10">
@@ -1489,29 +1520,29 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="2" t="str">
         <f>Flows!A11</f>
         <v>WN</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>30</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>30</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>30</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>30</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>30</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>30</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>30</v>
       </c>
       <c r="I11">
@@ -1519,29 +1550,29 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="str">
+      <c r="A12" s="2" t="str">
         <f>Flows!A12</f>
         <v>QV</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>9.3025699999999993</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>9.4033600000000011</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>9.5909699999999987</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>9.5640200000000011</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>9.0969999999999995</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>9.038120000000001</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>0</v>
       </c>
       <c r="I12">
@@ -1549,29 +1580,29 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="2" t="str">
         <f>Flows!A13</f>
         <v>QG</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>2.1219999999999999</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>2.23</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>2.1560000000000001</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>2.1120000000000001</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>2.2280000000000002</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>2.3530000000000002</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>14.784000000000001</v>
       </c>
       <c r="I13">
@@ -1589,113 +1620,115 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="28" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="10">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1705,7 +1738,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,19 +1747,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2">_xlfn._xlws.FILTER(Flows!A2:A13,Flows!B2:B13="WASTE")</f>
+        <v>QG</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1758,16 +1792,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1775,7 +1809,7 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>0.76800000000000002</v>
       </c>
     </row>
@@ -1783,7 +1817,7 @@
       <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
@@ -1791,7 +1825,7 @@
       <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.05</v>
       </c>
     </row>
@@ -1799,7 +1833,7 @@
       <c r="A5" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
@@ -1810,36 +1844,40 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>55</v>
+      <c r="A2" t="str">
+        <f>Flows!A2</f>
+        <v>NG</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>30</v>
       </c>
       <c r="D2">
@@ -1848,13 +1886,14 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
+      <c r="A3" t="str">
+        <f>Processes!A2</f>
+        <v>COMB</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>3.6</v>
       </c>
       <c r="D3">
@@ -1863,13 +1902,14 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>69</v>
+      <c r="A4" t="str">
+        <f>Processes!A3</f>
+        <v>CMP</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>32.5</v>
       </c>
       <c r="D4">
@@ -1878,13 +1918,14 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
+      <c r="A5" t="str">
+        <f>Processes!A4</f>
+        <v>TRB</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>46</v>
       </c>
       <c r="D5">
@@ -1893,13 +1934,14 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
+      <c r="A6" t="str">
+        <f>Processes!A5</f>
+        <v>APH</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>20</v>
       </c>
       <c r="D6">
@@ -1908,16 +1950,32 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
+      <c r="A7" t="str">
+        <f>Processes!A6</f>
+        <v>HRSG</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>35</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>Processes!A7</f>
+        <v>STCK</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0</v>
       </c>
     </row>

</xml_diff>